<commit_message>
added chlorophyll A to xlsx file
</commit_message>
<xml_diff>
--- a/data-raw/Chem_parameter_lookup.xlsx
+++ b/data-raw/Chem_parameter_lookup.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joe/Code/nrp/nrp/data-raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA58DA6-1183-3946-99A0-79A99D683874}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12780"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="32920" windowHeight="27240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMS.names" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="245">
   <si>
     <t>PARAMETER_CODE</t>
   </si>
@@ -740,13 +746,22 @@
   </si>
   <si>
     <t>calculated from TDP..mg.L.</t>
+  </si>
+  <si>
+    <t>0143</t>
+  </si>
+  <si>
+    <t>Chlorophyll A</t>
+  </si>
+  <si>
+    <t>﻿Colorimetric: Extraction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1224,7 +1239,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1253,6 +1268,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1304,6 +1321,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1351,7 +1371,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1384,9 +1404,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1419,6 +1456,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1594,23 +1648,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1629,8 +1683,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:6">
+      <c r="A2" s="28">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -1649,8 +1703,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:6">
+      <c r="A3" s="28">
         <v>15</v>
       </c>
       <c r="B3" t="s">
@@ -1669,8 +1723,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:6">
+      <c r="A4" s="28">
         <v>102</v>
       </c>
       <c r="B4" t="s">
@@ -1689,8 +1743,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:6">
+      <c r="A5" s="28">
         <v>103</v>
       </c>
       <c r="B5" t="s">
@@ -1709,8 +1763,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:6">
+      <c r="A6" s="28">
         <v>108</v>
       </c>
       <c r="B6" t="s">
@@ -1729,8 +1783,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:6">
+      <c r="A7" s="28">
         <v>114</v>
       </c>
       <c r="B7" t="s">
@@ -1749,8 +1803,8 @@
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:6">
+      <c r="A8" s="28">
         <v>124</v>
       </c>
       <c r="B8" t="s">
@@ -1769,747 +1823,751 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:6">
+      <c r="A9" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="28">
         <v>1109</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1110</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>188</v>
+      <c r="D10" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1111</v>
+    <row r="11" spans="1:6">
+      <c r="A11" s="28">
+        <v>1110</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>190</v>
+      <c r="D11" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>188</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1118</v>
+    <row r="12" spans="1:6">
+      <c r="A12" s="28">
+        <v>1111</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>207</v>
+        <v>18</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>190</v>
       </c>
       <c r="F12" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1120</v>
+    <row r="13" spans="1:6">
+      <c r="A13" s="28">
+        <v>1118</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>219</v>
+        <v>22</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>207</v>
       </c>
       <c r="F13" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
+    <row r="14" spans="1:6">
+      <c r="A14" s="28">
+        <v>1120</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>219</v>
+      </c>
       <c r="F14" s="27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="27" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:6">
+      <c r="A17" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="28">
         <v>107</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>27</v>
       </c>
-      <c r="F17" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="F18" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="28">
         <v>1107</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F19" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="F20" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="F21" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="F22" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="F23" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="F24" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>42</v>
       </c>
-      <c r="F24" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="F25" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>52</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="F26" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="F27" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>56</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="F28" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>58</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="F29" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>60</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="F30" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="F31" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>64</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="F32" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>66</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="F33" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>68</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="F34" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>70</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="F35" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>72</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="F36" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>74</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="F37" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>76</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="F38" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>78</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="F39" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>80</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="F40" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>82</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>42</v>
       </c>
-      <c r="F40" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="F41" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>84</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="F42" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>86</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>42</v>
       </c>
-      <c r="F42" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="F43" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>88</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>89</v>
       </c>
-      <c r="F43" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="F44" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>91</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>92</v>
       </c>
-      <c r="F44" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="F45" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>94</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="F46" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>96</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>42</v>
       </c>
-      <c r="F46" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="F47" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>98</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>39</v>
       </c>
-      <c r="F47" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="F48" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>100</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="F49" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>102</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>39</v>
       </c>
-      <c r="F49" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="F50" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>104</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>42</v>
       </c>
-      <c r="F50" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="F51" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>106</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>39</v>
       </c>
-      <c r="F51" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="F52" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>108</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>42</v>
       </c>
-      <c r="F52" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="F53" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>110</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>39</v>
       </c>
-      <c r="F53" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="F54" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>112</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>42</v>
       </c>
-      <c r="F54" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="F55" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>114</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>39</v>
       </c>
-      <c r="F55" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="F56" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>116</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>42</v>
       </c>
-      <c r="F56" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="F57" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -2517,362 +2575,364 @@
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:6">
+      <c r="A59" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>118</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>39</v>
       </c>
-      <c r="F59" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="F60" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>120</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>42</v>
       </c>
-      <c r="F60" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="F61" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>122</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="F62" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>124</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>42</v>
       </c>
-      <c r="F62" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="F63" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>126</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>39</v>
       </c>
-      <c r="F63" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="F64" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>128</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>42</v>
       </c>
-      <c r="F64" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="F65" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>130</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>39</v>
       </c>
-      <c r="F65" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="F66" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>132</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>42</v>
       </c>
-      <c r="F66" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="F67" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>134</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>39</v>
       </c>
-      <c r="F67" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="F68" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>136</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>42</v>
       </c>
-      <c r="F68" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="F69" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>138</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="F70" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>140</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>42</v>
       </c>
-      <c r="F70" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="F71" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>142</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>39</v>
       </c>
-      <c r="F71" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="F72" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>144</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>42</v>
       </c>
-      <c r="F72" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="F73" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>146</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>39</v>
       </c>
-      <c r="F73" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="F74" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>148</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>42</v>
       </c>
-      <c r="F74" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="F75" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>150</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>39</v>
       </c>
-      <c r="F75" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="F76" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>152</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>42</v>
       </c>
-      <c r="F76" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="F77" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>154</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>39</v>
       </c>
-      <c r="F77" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="F78" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>156</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" t="s">
         <v>42</v>
       </c>
-      <c r="F78" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="F79" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>158</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>39</v>
       </c>
-      <c r="F79" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="F80" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>160</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>42</v>
       </c>
-      <c r="F80" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="F81" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>162</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>39</v>
       </c>
-      <c r="F81" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="F82" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>164</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>42</v>
       </c>
-      <c r="F82" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83">
+      <c r="F83" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="28">
         <v>101</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>165</v>
-      </c>
-      <c r="C83" t="s">
-        <v>8</v>
-      </c>
-      <c r="F83" s="27" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>149</v>
-      </c>
-      <c r="B84" t="s">
-        <v>166</v>
       </c>
       <c r="C84" t="s">
         <v>8</v>
@@ -2881,12 +2941,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>150</v>
+    <row r="85" spans="1:6">
+      <c r="A85" s="28">
+        <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C85" t="s">
         <v>8</v>
@@ -2895,12 +2955,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>168</v>
+    <row r="86" spans="1:6">
+      <c r="A86" s="28">
+        <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C86" t="s">
         <v>8</v>
@@ -2909,28 +2969,22 @@
         <v>233</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>182</v>
+    <row r="87" spans="1:6">
+      <c r="A87" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="B87" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C87" t="s">
-        <v>182</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F87" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" s="27" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B88" s="8" t="s">
@@ -2949,8 +3003,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="20" t="s">
+    <row r="89" spans="1:6">
+      <c r="A89" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B89" s="20" t="s">
@@ -2969,8 +3023,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="20" t="s">
+    <row r="90" spans="1:6">
+      <c r="A90" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B90" s="20" t="s">
@@ -2989,8 +3043,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="20" t="s">
+    <row r="91" spans="1:6">
+      <c r="A91" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B91" s="20" t="s">
@@ -3009,8 +3063,8 @@
         <v>236</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="20" t="s">
+    <row r="92" spans="1:6">
+      <c r="A92" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B92" s="20" t="s">
@@ -3029,8 +3083,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="20" t="s">
+    <row r="93" spans="1:6">
+      <c r="A93" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B93" s="20" t="s">
@@ -3049,8 +3103,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="20" t="s">
+    <row r="94" spans="1:6">
+      <c r="A94" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B94" s="20" t="s">
@@ -3069,8 +3123,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="20" t="s">
+    <row r="95" spans="1:6">
+      <c r="A95" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B95" s="20" t="s">
@@ -3089,8 +3143,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="20" t="s">
+    <row r="96" spans="1:6">
+      <c r="A96" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B96" s="20" t="s">
@@ -3109,8 +3163,8 @@
         <v>240</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="26" t="s">
+    <row r="97" spans="1:6">
+      <c r="A97" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B97" s="26" t="s">
@@ -3129,8 +3183,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="26" t="s">
+    <row r="98" spans="1:6">
+      <c r="A98" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B98" s="26" t="s">
@@ -3149,8 +3203,8 @@
         <v>223</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="26" t="s">
+    <row r="99" spans="1:6">
+      <c r="A99" s="28" t="s">
         <v>182</v>
       </c>
       <c r="B99" s="26" t="s">

</xml_diff>